<commit_message>
2nd xgboost with new features
not good at all…
</commit_message>
<xml_diff>
--- a/features.xlsx
+++ b/features.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="22740" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="22740" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Original features" sheetId="1" r:id="rId1"/>
@@ -610,9 +610,6 @@
     <t>age groups…??? (the higher ps_ind_03, the higher ps_ind_01; and insurance claim rate is higher on two sides)</t>
   </si>
   <si>
-    <t>single or married or divorced? (something related to marriage, different group has different distribution of ps_ind_01)</t>
-  </si>
-  <si>
     <t>regional information; (4*ps_reg_03)^2 maps nicely to 2 decimal points</t>
   </si>
   <si>
@@ -740,6 +737,9 @@
   </si>
   <si>
     <t>ps_car_10_catnew</t>
+  </si>
+  <si>
+    <t>something related to marriage or gender, different group has different distribution of ps_ind_01</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1651,7 +1653,7 @@
         <v>152</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>193</v>
+        <v>236</v>
       </c>
       <c r="H19" s="23"/>
     </row>
@@ -1715,7 +1717,7 @@
         <v>146</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H22" s="17"/>
     </row>
@@ -1739,7 +1741,7 @@
         <v>148</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H23" s="17"/>
     </row>
@@ -1763,7 +1765,7 @@
         <v>148</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="33" t="s">
@@ -2066,7 +2068,7 @@
         <v>148</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H38" s="17"/>
       <c r="I38" s="33" t="s">
@@ -2672,7 +2674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2684,27 +2686,27 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="C1" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>200</v>
-      </c>
       <c r="F1" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="36" t="s">
         <v>199</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="36">
         <v>0.120632329802577</v>
@@ -2713,7 +2715,7 @@
         <v>3.6120401337792603E-2</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G2" s="36">
         <v>9.7592561975454295E-2</v>
@@ -2724,7 +2726,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B3" s="36">
         <v>9.6580350942298193E-2</v>
@@ -2733,7 +2735,7 @@
         <v>7.2201455833169406E-2</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="36">
         <v>9.4440315793511406E-2</v>
@@ -2753,7 +2755,7 @@
         <v>8.2825103285461305E-2</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G4" s="36">
         <v>8.5611897140312004E-2</v>
@@ -2764,7 +2766,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5" s="36">
         <v>7.8999485996748595E-2</v>
@@ -2844,7 +2846,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="36">
         <v>4.0101440973972599E-2</v>
@@ -2853,7 +2855,7 @@
         <v>4.0173126106629903E-2</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G9" s="36">
         <v>4.0680899462392797E-2</v>
@@ -2884,7 +2886,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="36">
         <v>2.9611237276546801E-2</v>
@@ -2893,7 +2895,7 @@
         <v>2.0735785953177301E-2</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G11" s="36">
         <v>3.0880625992805701E-2</v>
@@ -2913,7 +2915,7 @@
         <v>1.3850088530395399E-2</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G12" s="36">
         <v>3.0536310046132699E-2</v>
@@ -2924,7 +2926,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B13" s="36">
         <v>2.7928461432547201E-2</v>
@@ -2953,7 +2955,7 @@
         <v>3.0651190241983099E-2</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G14" s="36">
         <v>2.90287747421306E-2</v>
@@ -2964,7 +2966,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B15" s="36">
         <v>2.4585370602153302E-2</v>
@@ -2984,7 +2986,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B16" s="36">
         <v>2.1637308019255001E-2</v>
@@ -2993,7 +2995,7 @@
         <v>2.0775132795593201E-2</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G16" s="36">
         <v>2.5750528977297599E-2</v>
@@ -3004,7 +3006,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="36">
         <v>1.9924198988946401E-2</v>
@@ -3013,7 +3015,7 @@
         <v>2.1719457013574701E-2</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G17" s="36">
         <v>2.18046533747E-2</v>
@@ -3033,7 +3035,7 @@
         <v>1.03875663977966E-2</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G18" s="36">
         <v>2.0276820449275999E-2</v>
@@ -3044,7 +3046,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19" s="36">
         <v>1.6968616253064301E-2</v>
@@ -3053,7 +3055,7 @@
         <v>1.44402911666339E-2</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G19" s="36">
         <v>2.01365721718577E-2</v>
@@ -3104,7 +3106,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B22" s="36">
         <v>1.4858628545277501E-2</v>
@@ -3153,7 +3155,7 @@
         <v>7.7119811135156402E-3</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G24" s="36">
         <v>1.5200302979710501E-2</v>
@@ -3164,7 +3166,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25" s="36">
         <v>9.7120814682968605E-3</v>
@@ -3184,7 +3186,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B26" s="36">
         <v>6.62324875350575E-3</v>
@@ -3204,7 +3206,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B27" s="36">
         <v>6.5991751620626997E-3</v>
@@ -3224,7 +3226,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B28" s="36">
         <v>6.5419032646097299E-3</v>
@@ -3233,7 +3235,7 @@
         <v>1.3653354318316E-2</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G28" s="36">
         <v>7.3088622676073202E-3</v>
@@ -3244,7 +3246,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B29" s="36">
         <v>6.5264400130833396E-3</v>
@@ -3253,7 +3255,7 @@
         <v>1.03875663977966E-2</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G29" s="36">
         <v>7.1984428878303199E-3</v>
@@ -3284,7 +3286,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B31" s="36">
         <v>5.9850601319008899E-3</v>
@@ -3304,7 +3306,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B32" s="36">
         <v>5.9682791228028702E-3</v>
@@ -3313,7 +3315,7 @@
         <v>1.3377926421404699E-2</v>
       </c>
       <c r="F32" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G32" s="36">
         <v>3.8358565008798601E-3</v>
@@ -3333,7 +3335,7 @@
         <v>4.7216210899075402E-3</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G33" s="36">
         <v>3.02997996706484E-3</v>
@@ -3344,7 +3346,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B34" s="36">
         <v>4.25022861534165E-3</v>
@@ -3353,7 +3355,7 @@
         <v>9.0497737556561094E-3</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G34" s="36">
         <v>2.0106465263038599E-3</v>
@@ -3384,7 +3386,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B36" s="36">
         <v>3.3983931385380898E-3</v>
@@ -3393,7 +3395,7 @@
         <v>8.1841432225063897E-3</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G36" s="36">
         <v>9.0660238267665301E-4</v>
@@ -3404,7 +3406,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B37" s="36">
         <v>3.3193634548427898E-3</v>
@@ -3424,7 +3426,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B38" s="36">
         <v>2.9958170634246401E-3</v>
@@ -3433,7 +3435,7 @@
         <v>6.6496163682864496E-3</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G38" s="36">
         <v>1.99890227482499E-5</v>
@@ -3444,7 +3446,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B39" s="36">
         <v>2.6051528774008702E-3</v>
@@ -3455,7 +3457,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B40" s="36">
         <v>2.5536463479840701E-3</v>
@@ -3466,7 +3468,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B41" s="36">
         <v>2.2010983837218098E-3</v>
@@ -3477,7 +3479,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B42" s="36">
         <v>2.1348133636179701E-3</v>
@@ -3488,7 +3490,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B43" s="36">
         <v>1.67319349852983E-3</v>
@@ -3499,7 +3501,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B44" s="36">
         <v>1.65576517721324E-3</v>
@@ -3510,7 +3512,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B45" s="36">
         <v>1.4994221128844199E-3</v>
@@ -3521,7 +3523,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B46" s="36">
         <v>1.4288779529421901E-3</v>
@@ -3543,7 +3545,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B48" s="36">
         <v>7.9290725838822198E-4</v>
@@ -3554,7 +3556,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B49" s="36">
         <v>5.4844811853032097E-4</v>
@@ -3565,7 +3567,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B50" s="36">
         <v>3.2397407510044202E-4</v>
@@ -3576,7 +3578,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B51" s="36">
         <v>1.54725872793464E-4</v>
@@ -3587,7 +3589,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B52" s="36">
         <v>9.5637789908968197E-5</v>

</xml_diff>